<commit_message>
feat: Update Excel templates for barang, kategori, level, supplier, and user
</commit_message>
<xml_diff>
--- a/Semester4/PointOfSale/public/template_barang.xlsx
+++ b/Semester4/PointOfSale/public/template_barang.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vidoe\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233E8BA0-5AE0-4EDF-8B91-E948975AC2DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E7A9DC-46F2-4C43-9C92-C1453409A86F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,31 +20,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>No</t>
+    <t>Kategori_ID</t>
   </si>
   <si>
-    <t>Kode Barang</t>
+    <t>Barang_Kode</t>
   </si>
   <si>
-    <t>Nama Barang</t>
+    <t>Barang_Nama</t>
   </si>
   <si>
-    <t>Harga Beli</t>
+    <t>Harga_Beli</t>
   </si>
   <si>
-    <t>Harga Jual</t>
-  </si>
-  <si>
-    <t>Kategori</t>
+    <t>Harga_Jual</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -52,6 +49,12 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -78,9 +81,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,21 +389,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F16"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -415,9 +419,10 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>